<commit_message>
added recovery dates for Papa 00003 moorings and GL525
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GP02HYPM_00003.xlsx
+++ b/deployment/Omaha_Cal_Info_GP02HYPM_00003.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="7380" windowWidth="29700" windowHeight="14415" activeTab="1"/>
+    <workbookView xWindow="10840" yWindow="3800" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +17,12 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -725,7 +725,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="200">
+  <cellStyleXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -926,6 +926,8 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1094,7 +1096,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="200">
+  <cellStyles count="202">
     <cellStyle name="Comma 2" xfId="62"/>
     <cellStyle name="Comma 2 2" xfId="63"/>
     <cellStyle name="Comma 2 2 2" xfId="64"/>
@@ -1139,6 +1141,7 @@
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
@@ -1173,6 +1176,7 @@
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="8"/>
     <cellStyle name="Hyperlink 2 2" xfId="71"/>
     <cellStyle name="Hyperlink 2 3" xfId="72"/>
@@ -1310,7 +1314,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1369,7 +1373,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1404,7 +1408,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1615,30 +1619,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="11" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" style="11" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="12.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="11" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" style="11" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="11" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="12" customFormat="1" ht="28">
       <c r="A1" s="56" t="s">
         <v>52</v>
       </c>
@@ -1676,7 +1680,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="23" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="23" customFormat="1">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1695,7 +1699,9 @@
       <c r="F2" s="27">
         <v>0.98472222222222217</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="34">
+        <v>42552</v>
+      </c>
       <c r="H2" s="26" t="s">
         <v>50</v>
       </c>
@@ -1718,51 +1724,51 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="23" customFormat="1">
       <c r="E3" s="32"/>
       <c r="F3" s="33"/>
       <c r="G3" s="32"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" customFormat="1">
       <c r="M4" s="55"/>
       <c r="N4" s="55"/>
     </row>
-    <row r="5" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" customFormat="1"/>
+    <row r="6" spans="1:14" customFormat="1"/>
+    <row r="7" spans="1:14" customFormat="1"/>
+    <row r="8" spans="1:14" customFormat="1"/>
+    <row r="9" spans="1:14" customFormat="1"/>
+    <row r="10" spans="1:14" s="23" customFormat="1">
       <c r="E10" s="32"/>
       <c r="F10" s="33"/>
       <c r="G10" s="32"/>
     </row>
-    <row r="11" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="23" customFormat="1">
       <c r="E11" s="32"/>
       <c r="F11" s="33"/>
       <c r="G11" s="32"/>
     </row>
-    <row r="12" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="23" customFormat="1">
       <c r="E12" s="32"/>
       <c r="F12" s="33"/>
       <c r="G12" s="32"/>
     </row>
-    <row r="13" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="23" customFormat="1">
       <c r="E13" s="32"/>
       <c r="F13" s="33"/>
       <c r="G13" s="32"/>
     </row>
-    <row r="14" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="23" customFormat="1">
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
       <c r="G14" s="32"/>
     </row>
-    <row r="15" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="23" customFormat="1">
       <c r="E15" s="32"/>
       <c r="F15" s="33"/>
       <c r="G15" s="32"/>
     </row>
-    <row r="16" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="23" customFormat="1">
       <c r="E16" s="32"/>
       <c r="F16" s="33"/>
       <c r="G16" s="32"/>
@@ -1782,30 +1788,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="15" customWidth="1"/>
-    <col min="10" max="13" width="10.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="48.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="3" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="15" customWidth="1"/>
+    <col min="10" max="13" width="10.6640625" style="3" customWidth="1"/>
     <col min="14" max="14" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="3"/>
+    <col min="15" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="20" customFormat="1" ht="28">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1834,7 +1840,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="20" customFormat="1">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -1845,7 +1851,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="21"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1901,7 +1907,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1934,7 @@
       </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1955,7 +1961,7 @@
       </c>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1984,7 +1990,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -2071,7 +2077,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="2"/>
       <c r="B11" s="41"/>
       <c r="C11" s="36"/>
@@ -2082,7 +2088,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -2137,7 +2143,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="2"/>
       <c r="B14" s="41"/>
       <c r="C14" s="36"/>
@@ -2147,7 +2153,7 @@
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="2"/>
       <c r="B17" s="41"/>
       <c r="C17" s="36"/>
@@ -2209,7 +2215,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="15"/>
     </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -2235,7 +2241,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="2"/>
       <c r="B20" s="41"/>
       <c r="C20" s="36"/>
@@ -2271,7 +2277,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="42" t="s">
         <v>48</v>
       </c>
@@ -2292,10 +2298,10 @@
       </c>
       <c r="I21" s="45"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
@@ -2351,7 +2357,7 @@
       </c>
       <c r="I24" s="14"/>
     </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -2378,7 +2384,7 @@
       </c>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -2405,7 +2411,7 @@
       </c>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
@@ -2493,7 +2499,7 @@
       </c>
       <c r="J29" s="15"/>
     </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
@@ -2523,7 +2529,7 @@
       </c>
       <c r="J30" s="15"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="2"/>
       <c r="B31" s="41"/>
       <c r="C31" s="36"/>
@@ -2535,7 +2541,7 @@
       <c r="I31" s="13"/>
       <c r="J31" s="45"/>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -2562,7 +2568,7 @@
       </c>
       <c r="J32" s="45"/>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
@@ -2589,7 +2595,7 @@
       </c>
       <c r="J33" s="15"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="A34" s="2"/>
       <c r="B34" s="41"/>
       <c r="C34" s="36"/>
@@ -2599,7 +2605,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
@@ -2626,7 +2632,7 @@
       </c>
       <c r="J35" s="15"/>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="2" t="s">
         <v>11</v>
       </c>
@@ -2653,7 +2659,7 @@
       </c>
       <c r="J36" s="15"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14">
       <c r="A37" s="2"/>
       <c r="B37" s="41"/>
       <c r="C37" s="36"/>
@@ -2663,7 +2669,7 @@
       <c r="G37" s="6"/>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -2689,7 +2695,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
@@ -2715,7 +2721,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14">
       <c r="A40" s="41"/>
       <c r="B40" s="41"/>
       <c r="C40" s="36"/>
@@ -2725,7 +2731,7 @@
       <c r="G40" s="14"/>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14">
       <c r="A41" s="42" t="s">
         <v>49</v>
       </c>
@@ -2746,10 +2752,10 @@
       </c>
       <c r="I41" s="45"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14">
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14">
       <c r="A43" s="49" t="s">
         <v>44</v>
       </c>
@@ -2768,7 +2774,7 @@
       <c r="L43" s="39"/>
       <c r="N43" s="15"/>
     </row>
-    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="A44" s="49" t="s">
         <v>45</v>
       </c>
@@ -2787,7 +2793,7 @@
       <c r="L44" s="39"/>
       <c r="N44" s="15"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
       <c r="C45" s="35"/>
@@ -2795,7 +2801,7 @@
       <c r="H45" s="15"/>
       <c r="I45" s="40"/>
     </row>
-    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="A46" s="42" t="s">
         <v>46</v>
       </c>
@@ -2822,7 +2828,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="A47" s="42" t="s">
         <v>47</v>
       </c>
@@ -2848,7 +2854,7 @@
         <v>50.079833333333333</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="A48" s="42" t="s">
         <v>47</v>
       </c>
@@ -2874,7 +2880,7 @@
         <v>-144.803</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="41"/>
       <c r="B49" s="41"/>
       <c r="C49" s="36"/>
@@ -2884,7 +2890,7 @@
       <c r="G49" s="7"/>
       <c r="H49" s="15"/>
     </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="58" t="s">
         <v>69</v>
       </c>
@@ -2906,7 +2912,7 @@
       <c r="G50" s="44"/>
       <c r="H50" s="44"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="42"/>
       <c r="B51" s="42"/>
       <c r="D51" s="3"/>
@@ -2918,5 +2924,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>